<commit_message>
FINALLY updating the TOR330 code, working on TOR450 cleaning and prepping
</commit_message>
<xml_diff>
--- a/TOR330 Data/4. TOR330 Timetable Data/TOR330_aid_station_for_each_year_cut_offs_df.xlsx
+++ b/TOR330 Data/4. TOR330 Timetable Data/TOR330_aid_station_for_each_year_cut_offs_df.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="45">
   <si>
-    <t>Aid Station</t>
+    <t>Checkpoint</t>
   </si>
   <si>
     <t>Year</t>
@@ -25,7 +25,7 @@
     <t>Wave</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cut Off Date</t>
+    <t>Cut Off Date</t>
   </si>
   <si>
     <t>Stage</t>

</xml_diff>